<commit_message>
Add Form Design Sheet Class
</commit_message>
<xml_diff>
--- a/excel_doc/ApiDoc01.xlsx
+++ b/excel_doc/ApiDoc01.xlsx
@@ -1147,13 +1147,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>画面ID</t>
-    <rPh sb="0" eb="2">
-      <t>ガメン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>customerName</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1402,6 +1395,13 @@
     </rPh>
     <rPh sb="3" eb="5">
       <t>ネンゲツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>画面id</t>
+    <rPh sb="0" eb="2">
+      <t>ガメン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1810,7 +1810,7 @@
   <dimension ref="A1:G95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1830,7 +1830,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>138</v>
+        <v>174</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>20</v>
@@ -1840,13 +1840,13 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1901,109 +1901,109 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>134</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E8" s="1">
         <v>20</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>134</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E9" s="1">
         <v>8</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>134</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E10" s="1">
         <v>7</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>134</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E11" s="1">
         <v>256</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
@@ -2034,117 +2034,117 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>158</v>
-      </c>
       <c r="E16" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>165</v>
-      </c>
       <c r="E17" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F17" s="5">
         <v>3</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>166</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>167</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>134</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F18" s="5">
         <v>20</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>134</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F19" s="5">
         <v>6</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>171</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>134</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F20" s="5">
         <v>6</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Change ApiDoc01.xlsx and Fixed Comment.
</commit_message>
<xml_diff>
--- a/excel_doc/ApiDoc01.xlsx
+++ b/excel_doc/ApiDoc01.xlsx
@@ -1373,13 +1373,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>物理パス</t>
-    <rPh sb="0" eb="2">
-      <t>ブツリ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>p0101</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1416,37 +1409,47 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>業務id</t>
+    <t>業務</t>
     <rPh sb="0" eb="2">
       <t>ギョウム</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>業務</t>
+    <t>p0101</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>業務プログラムid</t>
     <rPh sb="0" eb="2">
       <t>ギョウム</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>業務名</t>
+    <t>業務プログラム名</t>
     <rPh sb="0" eb="2">
       <t>ギョウム</t>
     </rPh>
-    <rPh sb="2" eb="3">
+    <rPh sb="7" eb="8">
       <t>メイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>p0101</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>初期画面id</t>
-    <rPh sb="0" eb="4">
-      <t>ショキガメン</t>
+    <t>パス</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>初期表示画面id</t>
+    <rPh sb="0" eb="2">
+      <t>ショキ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ガメン</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1865,15 +1868,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17.125" customWidth="1"/>
     <col min="2" max="3" width="21.125" customWidth="1"/>
-    <col min="4" max="4" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.375" bestFit="1" customWidth="1"/>
@@ -1881,18 +1884,18 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>178</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>180</v>
@@ -1900,16 +1903,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
@@ -1939,10 +1942,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>127</v>
@@ -1951,13 +1954,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D9" s="8"/>
     </row>
@@ -1997,7 +2000,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>132</v>
@@ -2020,7 +2023,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>136</v>
@@ -2043,7 +2046,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>140</v>
@@ -2066,7 +2069,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>138</v>
@@ -2089,7 +2092,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>142</v>
@@ -2112,7 +2115,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>145</v>

</xml_diff>

<commit_message>
Add Design Data Insert Process.
</commit_message>
<xml_diff>
--- a/excel_doc/ApiDoc01.xlsx
+++ b/excel_doc/ApiDoc01.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="182">
   <si>
     <t>リクエスト種別</t>
     <rPh sb="5" eb="7">
@@ -1409,13 +1409,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>業務</t>
-    <rPh sb="0" eb="2">
-      <t>ギョウム</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>p0101</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1437,10 +1430,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>パス</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>初期表示画面id</t>
     <rPh sb="0" eb="2">
       <t>ショキ</t>
@@ -1451,6 +1440,21 @@
     <rPh sb="4" eb="6">
       <t>ガメン</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>業務プログラム</t>
+    <rPh sb="0" eb="2">
+      <t>ギョウム</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>パス</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>g010101</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1869,7 +1873,7 @@
   <dimension ref="A1:G102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1884,21 +1888,21 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>178</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
@@ -1909,10 +1913,10 @@
         <v>131</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Change Excel Document Format
</commit_message>
<xml_diff>
--- a/excel_doc/ApiDoc01.xlsx
+++ b/excel_doc/ApiDoc01.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="205">
   <si>
     <t>リクエスト種別</t>
     <rPh sb="5" eb="7">
@@ -1469,10 +1469,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>body</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>階層内表示順</t>
     <rPh sb="0" eb="2">
       <t>カイソウ</t>
@@ -1605,15 +1601,14 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>height</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>width</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>-</t>
+    <t>readonly</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>g010101</t>
+  </si>
+  <si>
+    <t>g010101</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1657,7 +1652,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1698,11 +1693,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1712,6 +1718,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -2029,10 +2036,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U106"/>
+  <dimension ref="A1:V106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2046,12 +2053,12 @@
     <col min="11" max="11" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>175</v>
       </c>
@@ -2065,7 +2072,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>168</v>
       </c>
@@ -2079,20 +2086,20 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A5" s="7"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>167</v>
       </c>
@@ -2104,7 +2111,7 @@
       </c>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>171</v>
       </c>
@@ -2116,7 +2123,7 @@
       </c>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>172</v>
       </c>
@@ -2128,18 +2135,18 @@
       </c>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>167</v>
       </c>
@@ -2165,46 +2172,49 @@
         <v>181</v>
       </c>
       <c r="I13" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="K13" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="N13" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="M13" s="2" t="s">
+      <c r="O13" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="P13" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="N13" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="O13" s="2" t="s">
+      <c r="Q13" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="P13" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q13" s="2" t="s">
+      <c r="R13" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="R13" s="2" t="s">
+      <c r="S13" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="S13" s="2" t="s">
+      <c r="T13" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="T13" s="2" t="s">
+      <c r="U13" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="U13" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="V13" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>171</v>
       </c>
@@ -2241,7 +2251,7 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>171</v>
       </c>
@@ -2278,7 +2288,7 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>171</v>
       </c>
@@ -2454,430 +2464,469 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="G23" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="H23" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="I23" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="J23" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="K23" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="L23" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="M23" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="K23" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="M23" s="4" t="s">
-        <v>204</v>
-      </c>
       <c r="N23" s="4" t="s">
-        <v>203</v>
+        <v>187</v>
+      </c>
+      <c r="O23" s="4" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="1">
+      <c r="E24" s="5"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="1">
         <v>0</v>
       </c>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1">
+      <c r="K24" s="1"/>
+      <c r="L24" s="1">
         <v>0</v>
       </c>
-      <c r="L24" s="1">
+      <c r="M24" s="1">
         <v>1</v>
       </c>
-      <c r="M24" s="1">
+      <c r="N24" s="1">
         <v>50</v>
       </c>
-      <c r="N24" s="1">
+      <c r="O24" s="1">
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="1"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
-      <c r="I25" s="1">
+      <c r="I25" s="5"/>
+      <c r="J25" s="1">
         <v>0</v>
       </c>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1">
+      <c r="K25" s="1"/>
+      <c r="L25" s="1">
         <v>1</v>
       </c>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1">
+      <c r="M25" s="1"/>
+      <c r="N25" s="1">
         <v>50</v>
       </c>
-      <c r="N25" s="1" t="s">
-        <v>205</v>
+      <c r="O25" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="1"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
-      <c r="I26" s="1">
+      <c r="I26" s="5"/>
+      <c r="J26" s="1">
         <v>0</v>
       </c>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1">
+      <c r="K26" s="1"/>
+      <c r="L26" s="1">
         <v>2</v>
       </c>
-      <c r="L26" s="1"/>
       <c r="M26" s="1"/>
-      <c r="N26" s="1" t="s">
-        <v>205</v>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="1"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="1">
+      <c r="I27" s="5"/>
+      <c r="J27" s="1">
         <v>0</v>
       </c>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1">
+      <c r="K27" s="1"/>
+      <c r="L27" s="1">
         <v>3</v>
       </c>
-      <c r="L27" s="1"/>
       <c r="M27" s="1"/>
-      <c r="N27" s="1" t="s">
-        <v>205</v>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="1">
+      <c r="E28" s="5"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="1">
         <v>1</v>
       </c>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1">
+      <c r="K28" s="1"/>
+      <c r="L28" s="1">
         <v>0</v>
       </c>
-      <c r="L28" s="1">
+      <c r="M28" s="1">
         <v>1</v>
       </c>
-      <c r="M28" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="N28" s="1">
+      <c r="N28" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="O28" s="1">
         <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="1"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
-      <c r="I29" s="1">
+      <c r="I29" s="5"/>
+      <c r="J29" s="1">
         <v>1</v>
       </c>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1">
+      <c r="K29" s="1"/>
+      <c r="L29" s="1">
         <v>1</v>
       </c>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1" t="s">
-        <v>205</v>
-      </c>
+      <c r="M29" s="1"/>
       <c r="N29" s="1" t="s">
-        <v>205</v>
+        <v>152</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="1"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
-      <c r="I30" s="1">
+      <c r="I30" s="5"/>
+      <c r="J30" s="1">
         <v>1</v>
       </c>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1">
+      <c r="K30" s="1"/>
+      <c r="L30" s="1">
         <v>2</v>
       </c>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1" t="s">
-        <v>205</v>
-      </c>
+      <c r="M30" s="1"/>
       <c r="N30" s="1" t="s">
-        <v>205</v>
+        <v>152</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="1"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
-      <c r="I31" s="1">
+      <c r="I31" s="5"/>
+      <c r="J31" s="1">
         <v>1</v>
       </c>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1">
+      <c r="K31" s="1"/>
+      <c r="L31" s="1">
         <v>3</v>
       </c>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1" t="s">
-        <v>205</v>
-      </c>
+      <c r="M31" s="1"/>
       <c r="N31" s="1" t="s">
-        <v>205</v>
+        <v>152</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="D32" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="E32" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="F32" s="5">
+      <c r="G32" s="5">
         <v>3</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="I32" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="I32" s="1">
+      <c r="J32" s="1">
         <v>0</v>
       </c>
-      <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
-      <c r="N32" s="1">
+      <c r="N32" s="1"/>
+      <c r="O32" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="C33" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="D33" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="E33" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F33" s="5">
+      <c r="G33" s="5">
         <v>20</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="H33" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="I33" s="1"/>
+      <c r="I33" s="5" t="s">
+        <v>197</v>
+      </c>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
-      <c r="N33" s="1">
+      <c r="N33" s="1"/>
+      <c r="O33" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="C34" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="E34" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F34" s="5">
+      <c r="G34" s="5">
         <v>6</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="H34" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="I34" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
-      <c r="N34" s="1">
+      <c r="N34" s="1"/>
+      <c r="O34" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="C35" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="D35" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="E35" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="F35" s="5">
+      <c r="G35" s="5">
         <v>6</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="H35" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="H35" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="I35" s="1"/>
+      <c r="I35" s="5" t="s">
+        <v>183</v>
+      </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
-      <c r="N35" s="1">
+      <c r="N35" s="1"/>
+      <c r="O35" s="1">
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
     </row>
-    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.15"/>
-    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.15"/>
-    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.15"/>
+    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.15"/>
+    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
         <v>12</v>
       </c>
@@ -2888,7 +2937,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>27</v>
       </c>
@@ -2897,7 +2946,7 @@
       </c>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>28</v>
       </c>
@@ -2906,7 +2955,7 @@
       </c>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>

</xml_diff>